<commit_message>
Add trajectory column in replicate details
</commit_message>
<xml_diff>
--- a/det/DETAILSTEMPLATE.xlsx
+++ b/det/DETAILSTEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas03/Library/CloudStorage/OneDrive-CRUKCambridgeInstitute/ddrcs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/group_folders/sl681/bio/Projects/operation/crispr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72796A28-A0E6-B94A-A047-EA96090356D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C6A0DF-F5D6-4244-BAD3-DF29E4C0F761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="14960" windowWidth="33500" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="36860" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <author>John C. Thomas</author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{EC856BF7-5DB3-4FE4-84EE-8DB9186945B6}">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{EC856BF7-5DB3-4FE4-84EE-8DB9186945B6}">
       <text>
         <r>
           <rPr>
@@ -81,6 +81,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>John C. Thomas</author>
+    <author>tc={E0B596C2-2CB3-4048-85CB-8D7E46F3D407}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A2C7780A-B8D1-3C47-BF2B-F2B83A85B697}">
@@ -123,7 +124,15 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{DF922E7A-61BE-DE4D-B528-0CA06AE3812B}">
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{E0B596C2-2CB3-4048-85CB-8D7E46F3D407}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    For Chronos analysis. Give all samples that are on the same growth trajectory the same value in this column</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{DF922E7A-61BE-DE4D-B528-0CA06AE3812B}">
       <text>
         <r>
           <rPr>
@@ -210,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Library</t>
   </si>
@@ -317,7 +326,25 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Required for screen viewer</t>
+    <t>In e.g. MLA format</t>
+  </si>
+  <si>
+    <t>Used as ID in database</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Full URL or just the numbers works</t>
+  </si>
+  <si>
+    <t>Use consistent names for the library, e.g. in Exorcise outputs.</t>
+  </si>
+  <si>
+    <t>Organism</t>
+  </si>
+  <si>
+    <t>Trajectory</t>
   </si>
 </sst>
 </file>
@@ -502,7 +529,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1093,22 +1139,29 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Simon Lam" id="{AFA46504-15C8-504E-AED1-C1F61E070D00}" userId="S::sl681@cam.ac.uk::5c283c04-bc5b-491c-b42b-3f2e7d1aedb5" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}" name="samp_deets2" displayName="samp_deets2" ref="A1:L11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:L11" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}" name="samp_deets2" displayName="samp_deets2" ref="A1:M11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:M11" xr:uid="{E0A63A21-9CD2-8D4F-871C-3B6CE038B02C}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{4A7B1510-870A-E341-BD37-430A1066E449}" name="Replicate"/>
     <tableColumn id="2" xr3:uid="{8287588F-8FD3-A646-94D4-43B56F35F2DB}" name="Sample"/>
-    <tableColumn id="3" xr3:uid="{349D7A1F-9830-4C45-8AEF-C7842342C8FF}" name="Label" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{98385D66-7ED3-7749-80A3-94C7E96E4451}" name="Treatment" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{52166F07-06B2-404F-A476-58B2DB13078C}" name="Dose" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{ED651564-84AB-EF4D-AC19-AF0345918764}" name="Growth inhibition %" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{D241A1B9-B2EA-CE47-9E53-EBF0981EBAC4}" name="Days grown" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{175C51C1-979B-3A47-B7CF-FBBA4D85DB6F}" name="Doublings" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{67C7EB45-33AD-D543-B5E9-19070BE9652F}" name="Clone" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{64051FFB-C55B-3E4E-8589-AF512E28AA60}" name="Cell line" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{97C52B05-0225-BE45-A58B-1C32FFD7DC11}" name="KO" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{60C18679-5B03-2049-AEEB-5B6CFE4800AF}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{349D7A1F-9830-4C45-8AEF-C7842342C8FF}" name="Label" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{98385D66-7ED3-7749-80A3-94C7E96E4451}" name="Treatment" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{52166F07-06B2-404F-A476-58B2DB13078C}" name="Dose" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{ED651564-84AB-EF4D-AC19-AF0345918764}" name="Growth inhibition %" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{D241A1B9-B2EA-CE47-9E53-EBF0981EBAC4}" name="Days grown" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{175C51C1-979B-3A47-B7CF-FBBA4D85DB6F}" name="Doublings" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{F9000F6D-8BFF-6E49-AA2D-ADCF586A81C1}" name="Trajectory" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{67C7EB45-33AD-D543-B5E9-19070BE9652F}" name="Clone" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{64051FFB-C55B-3E4E-8589-AF512E28AA60}" name="Cell line" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{97C52B05-0225-BE45-A58B-1C32FFD7DC11}" name="KO" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{60C18679-5B03-2049-AEEB-5B6CFE4800AF}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1399,11 +1452,19 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I1" dT="2025-07-07T09:47:04.76" personId="{AFA46504-15C8-504E-AED1-C1F61E070D00}" id="{E0B596C2-2CB3-4048-85CB-8D7E46F3D407}">
+    <text>For Chronos analysis. Give all samples that are on the same growth trajectory the same value in this column</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059C090B-B234-4A49-8DCA-8601C4271810}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1416,10 +1477,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1433,12 +1494,18 @@
         <v>15</v>
       </c>
       <c r="B1" s="10"/>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="20">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="11"/>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="20">
       <c r="A3" s="1" t="s">
@@ -1446,7 +1513,7 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20">
@@ -1463,38 +1530,50 @@
     </row>
     <row r="6" spans="1:3" ht="20">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="7" spans="1:3" ht="20">
       <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="20">
       <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="12"/>
-    </row>
-    <row r="9" spans="1:3" ht="21" thickBot="1">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" thickBot="1">
+      <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Alphanumeric only" error="Alphanumeric only." sqref="B1" xr:uid="{50DA87F9-C9A8-AD4D-851D-DCA4B42EAA51}">
-      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(B1,ROW(INDIRECT("1:"&amp;LEN(B1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
+      <formula1>ISNUMBER(SUMPRODUCT(SEARCH(MID(B1,ROW(INDIRECT("1:"&amp;LEN(B1))),1),"_0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ")))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1505,11 +1584,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -1520,13 +1597,13 @@
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="8" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20">
+    <row r="1" spans="1:13" ht="20">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1551,20 +1628,23 @@
       <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="22" customHeight="1">
+    <row r="2" spans="1:13" ht="22" customHeight="1">
       <c r="B2" s="9"/>
       <c r="C2" s="2"/>
       <c r="E2" s="7"/>
@@ -1572,8 +1652,9 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" ht="19">
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="19">
       <c r="B3" s="9"/>
       <c r="C3" s="2"/>
       <c r="E3" s="7"/>
@@ -1581,8 +1662,9 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" ht="19">
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" ht="19">
       <c r="B4" s="9"/>
       <c r="C4" s="2"/>
       <c r="E4" s="7"/>
@@ -1590,8 +1672,9 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" ht="19">
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" ht="19">
       <c r="B5" s="9"/>
       <c r="C5" s="2"/>
       <c r="E5" s="7"/>
@@ -1599,8 +1682,9 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" ht="19">
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" ht="19">
       <c r="B6" s="9"/>
       <c r="C6" s="2"/>
       <c r="E6" s="7"/>
@@ -1608,8 +1692,9 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="19">
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="19">
       <c r="B7" s="9"/>
       <c r="C7" s="2"/>
       <c r="E7" s="7"/>
@@ -1617,8 +1702,9 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="19">
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="19">
       <c r="B8" s="9"/>
       <c r="C8" s="2"/>
       <c r="E8" s="7"/>
@@ -1626,8 +1712,9 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" ht="19">
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="19">
       <c r="B9" s="9"/>
       <c r="C9" s="2"/>
       <c r="E9" s="7"/>
@@ -1635,8 +1722,9 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="19">
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="19">
       <c r="B10" s="9"/>
       <c r="C10" s="2"/>
       <c r="E10" s="7"/>
@@ -1644,8 +1732,9 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="19">
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" ht="19">
       <c r="B11" s="9"/>
       <c r="C11" s="2"/>
       <c r="E11" s="7"/>
@@ -1653,6 +1742,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1682,7 +1772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5852547F-8F24-4C5C-A576-33824D0B5E92}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>

</xml_diff>